<commit_message>
Glucose logging staff dashboard
</commit_message>
<xml_diff>
--- a/Documentation/Work Plan.xlsx
+++ b/Documentation/Work Plan.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Documents\University\Nightingale Project\Git Nightingale\Nightingale\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB1EC03-2ADA-4183-B351-51B0AD90E899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24163714-98B7-4012-9ACA-9D829AF70A70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{4E11A371-AA18-4E58-9B7E-B7FAD8BE85E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Tasks &amp; Deadlines" sheetId="1" r:id="rId1"/>
     <sheet name="Easy Glance Planner" sheetId="4" r:id="rId2"/>
-    <sheet name="Project Plan (Initial)" sheetId="3" r:id="rId3"/>
-    <sheet name="Project Plan (Ongoing)" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Project Plan (Initial)" sheetId="3" r:id="rId4"/>
+    <sheet name="Project Plan (Ongoing)" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="152">
   <si>
     <t>Date</t>
   </si>
@@ -402,9 +402,6 @@
     <t>Final Year Project</t>
   </si>
   <si>
-    <t>Web app Intergration</t>
-  </si>
-  <si>
     <t>Team Project</t>
   </si>
   <si>
@@ -463,6 +460,39 @@
   </si>
   <si>
     <t>Glucose level Logging + Staff Panic button</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reading </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select data </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Staff Login System</t>
+  </si>
+  <si>
+    <t>Team Project report</t>
+  </si>
+  <si>
+    <t>staff login + Admin Dashboard</t>
+  </si>
+  <si>
+    <t>team project report</t>
+  </si>
+  <si>
+    <t>Diss 2000w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diss 2000w </t>
+  </si>
+  <si>
+    <t>Finish app</t>
+  </si>
+  <si>
+    <t>Finish app - PDO prepare for all SQL - info screens (text to speach)</t>
   </si>
 </sst>
 </file>
@@ -534,7 +564,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -598,12 +628,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -957,8 +981,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1299,20 +1323,20 @@
       <selection pane="topRight" activeCell="EI9" sqref="EI9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
-    <col min="3" max="3" width="23.81640625" customWidth="1"/>
-    <col min="4" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="39" width="26.81640625" customWidth="1"/>
-    <col min="40" max="75" width="25.26953125" customWidth="1"/>
-    <col min="76" max="94" width="23.26953125" customWidth="1"/>
-    <col min="95" max="132" width="27.453125" customWidth="1"/>
-    <col min="133" max="187" width="27.26953125" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="39" width="26.85546875" customWidth="1"/>
+    <col min="40" max="75" width="25.28515625" customWidth="1"/>
+    <col min="76" max="94" width="23.28515625" customWidth="1"/>
+    <col min="95" max="132" width="27.42578125" customWidth="1"/>
+    <col min="133" max="187" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:187" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:187" s="5" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +1896,7 @@
         <v>43946</v>
       </c>
     </row>
-    <row r="3" spans="2:187" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:187" s="5" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
@@ -2432,7 +2456,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:187" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:187" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>12</v>
       </c>
@@ -2634,7 +2658,7 @@
       <c r="GD4" s="2"/>
       <c r="GE4" s="2"/>
     </row>
-    <row r="5" spans="2:187" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:187" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
         <v>1</v>
       </c>
@@ -2903,7 +2927,7 @@
       <c r="GD5" s="2"/>
       <c r="GE5" s="2"/>
     </row>
-    <row r="6" spans="2:187" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:187" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
         <v>19</v>
       </c>
@@ -3110,7 +3134,7 @@
       <c r="GD6" s="2"/>
       <c r="GE6" s="2"/>
     </row>
-    <row r="7" spans="2:187" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:187" s="1" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>2</v>
       </c>
@@ -3368,7 +3392,7 @@
       <c r="GD7" s="3"/>
       <c r="GE7" s="3"/>
     </row>
-    <row r="8" spans="2:187" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:187" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>11</v>
       </c>
@@ -3586,21 +3610,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B88F32-7544-4375-8853-40EE08DCAD6D}">
   <dimension ref="B2:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.81640625" customWidth="1"/>
-    <col min="5" max="5" width="1.26953125" customWidth="1"/>
-    <col min="6" max="6" width="70.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="1.28515625" customWidth="1"/>
+    <col min="6" max="6" width="70.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="66" t="s">
         <v>110</v>
       </c>
@@ -3615,147 +3639,147 @@
         <v>111</v>
       </c>
       <c r="G2" s="66" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" s="66" t="s">
         <v>130</v>
       </c>
-      <c r="H2" s="66" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="68">
         <v>43910</v>
       </c>
       <c r="C3" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="E3" s="73"/>
+      <c r="E3" s="72"/>
       <c r="F3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G3" s="70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H3" s="70" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="68">
         <v>43911</v>
       </c>
       <c r="C4" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="73"/>
+      <c r="E4" s="72"/>
       <c r="F4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G4" s="70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H4" s="70" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="68">
         <v>43912</v>
       </c>
       <c r="C5" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="73"/>
+      <c r="E5" s="72"/>
       <c r="F5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G5" s="70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H5" s="70" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="68">
         <v>43913</v>
       </c>
       <c r="C6" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="73"/>
+      <c r="E6" s="72"/>
       <c r="F6" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="68">
         <v>43914</v>
       </c>
       <c r="C7" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="73"/>
+      <c r="E7" s="72"/>
       <c r="F7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G7" s="70" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="68">
         <v>43915</v>
       </c>
       <c r="C8" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="73"/>
+      <c r="E8" s="72"/>
       <c r="F8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G8" s="34"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="68">
         <v>43916</v>
       </c>
       <c r="C9" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="73"/>
+      <c r="E9" s="72"/>
       <c r="F9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G9" s="34"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="68">
         <v>43917</v>
       </c>
       <c r="C10" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="E10" s="73"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="E10" s="72"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="68">
         <v>43918</v>
       </c>
       <c r="C11" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="73"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="E11" s="72"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="68">
         <v>43919</v>
       </c>
       <c r="C12" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="E12" s="73"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="E12" s="72"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="68">
         <v>43920</v>
       </c>
@@ -3763,160 +3787,160 @@
         <v>116</v>
       </c>
       <c r="F13" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="68">
         <v>43921</v>
       </c>
       <c r="C14" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E14" s="73"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="E14" s="72"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="68">
         <v>43922</v>
       </c>
       <c r="C15" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="E15" s="73"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="E15" s="72"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="68">
         <v>43923</v>
       </c>
       <c r="C16" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="E16" s="73"/>
+      <c r="E16" s="72"/>
       <c r="F16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="68">
         <v>43924</v>
       </c>
       <c r="C17" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="E17" s="73"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E17" s="72"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="68">
         <v>43925</v>
       </c>
       <c r="C18" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="E18" s="73"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E18" s="72"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" s="68">
         <v>43926</v>
       </c>
       <c r="C19" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="73"/>
+      <c r="E19" s="72"/>
       <c r="F19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="68">
         <v>43927</v>
       </c>
       <c r="C20" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="73"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E20" s="72"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="68">
         <v>43928</v>
       </c>
       <c r="C21" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E21" s="73"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E21" s="72"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="68">
         <v>43929</v>
       </c>
       <c r="C22" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="73"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E22" s="72"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="68">
         <v>43930</v>
       </c>
       <c r="C23" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="E23" s="73"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E23" s="72"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="68">
         <v>43931</v>
       </c>
       <c r="C24" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="E24" s="73"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E24" s="72"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="68">
         <v>43932</v>
       </c>
       <c r="C25" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="E25" s="73"/>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E25" s="72"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="68">
         <v>43933</v>
       </c>
       <c r="C26" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="E26" s="73"/>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E26" s="72"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="68">
         <v>43934</v>
       </c>
       <c r="C27" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="E27" s="73"/>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E27" s="72"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" s="68">
         <v>43935</v>
       </c>
       <c r="C28" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E28" s="73"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E28" s="72"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" s="68">
         <v>43936</v>
       </c>
       <c r="C29" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="E29" s="73"/>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E29" s="72"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" s="68">
         <v>43937</v>
       </c>
@@ -3925,7 +3949,7 @@
       </c>
       <c r="E30" s="71"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" s="68">
         <v>43938</v>
       </c>
@@ -3934,7 +3958,7 @@
       </c>
       <c r="E31" s="71"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B32" s="68">
         <v>43939</v>
       </c>
@@ -3943,7 +3967,7 @@
       </c>
       <c r="E32" s="71"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="68">
         <v>43940</v>
       </c>
@@ -3952,7 +3976,7 @@
       </c>
       <c r="E33" s="71"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="68">
         <v>43941</v>
       </c>
@@ -3960,11 +3984,11 @@
         <v>116</v>
       </c>
       <c r="D34" s="71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E34" s="71"/>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="68">
         <v>43942</v>
       </c>
@@ -3972,10 +3996,10 @@
         <v>117</v>
       </c>
       <c r="F35" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="68">
         <v>43943</v>
       </c>
@@ -3984,61 +4008,61 @@
       </c>
       <c r="E36" s="71"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="68">
         <v>43944</v>
       </c>
       <c r="C37" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="E37" s="73"/>
+      <c r="E37" s="72"/>
       <c r="F37" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="68">
         <v>43945</v>
       </c>
       <c r="C38" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="E38" s="73"/>
+      <c r="E38" s="72"/>
       <c r="F38" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="68">
         <v>43946</v>
       </c>
       <c r="C39" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="E39" s="73"/>
+      <c r="E39" s="72"/>
       <c r="F39" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="68">
         <v>43947</v>
       </c>
       <c r="C40" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="E40" s="73"/>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E40" s="72"/>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="68">
         <v>43948</v>
       </c>
       <c r="C41" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="73"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E41" s="72"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="68">
         <v>43949</v>
       </c>
@@ -4047,7 +4071,7 @@
       </c>
       <c r="E42" s="69"/>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="68">
         <v>43950</v>
       </c>
@@ -4056,7 +4080,7 @@
       </c>
       <c r="E43" s="69"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="68">
         <v>43951</v>
       </c>
@@ -4065,7 +4089,7 @@
       </c>
       <c r="E44" s="69"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="68">
         <v>43952</v>
       </c>
@@ -4077,7 +4101,7 @@
       </c>
       <c r="E45" s="69"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="68">
         <v>43953</v>
       </c>
@@ -4085,10 +4109,10 @@
         <v>114</v>
       </c>
       <c r="F46" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="68">
         <v>43954</v>
       </c>
@@ -4096,126 +4120,130 @@
         <v>115</v>
       </c>
       <c r="F47" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="68">
         <v>43955</v>
       </c>
       <c r="C48" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="E48" s="73"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E48" s="72"/>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="68">
         <v>43956</v>
       </c>
       <c r="C49" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E49" s="73"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E49" s="72"/>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="68">
         <v>43957</v>
       </c>
       <c r="C50" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="E50" s="73"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E50" s="72"/>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="68">
         <v>43958</v>
       </c>
       <c r="C51" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="E51" s="73"/>
+      <c r="E51" s="72"/>
       <c r="F51" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="68">
         <v>43959</v>
       </c>
       <c r="C52" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="E52" s="73"/>
+      <c r="E52" s="72"/>
       <c r="F52" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="68">
         <v>43960</v>
       </c>
       <c r="C53" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="E53" s="73"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E53" s="72"/>
+      <c r="F53" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="68">
         <v>43961</v>
       </c>
       <c r="C54" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="E54" s="73"/>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E54" s="72"/>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="68">
         <v>43962</v>
       </c>
       <c r="C55" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="E55" s="73"/>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E55" s="72"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="68">
         <v>43963</v>
       </c>
       <c r="C56" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="E56" s="73"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E56" s="72"/>
+      <c r="F56" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="68">
         <v>43964</v>
       </c>
       <c r="C57" s="67" t="s">
         <v>118</v>
       </c>
-      <c r="E57" s="73"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E57" s="72"/>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="68">
         <v>43965</v>
       </c>
       <c r="C58" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="D58" s="73" t="s">
-        <v>120</v>
-      </c>
-      <c r="E58" s="73"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E58" s="72"/>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="68">
         <v>43966</v>
       </c>
       <c r="C59" s="67" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="E59" s="72"/>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="68">
         <v>43967</v>
       </c>
@@ -4224,7 +4252,7 @@
       </c>
       <c r="E60" s="72"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="68">
         <v>43968</v>
       </c>
@@ -4233,7 +4261,7 @@
       </c>
       <c r="E61" s="72"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="68">
         <v>43969</v>
       </c>
@@ -4242,7 +4270,7 @@
       </c>
       <c r="E62" s="72"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="68">
         <v>43970</v>
       </c>
@@ -4251,7 +4279,7 @@
       </c>
       <c r="E63" s="72"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="68">
         <v>43971</v>
       </c>
@@ -4260,7 +4288,7 @@
       </c>
       <c r="E64" s="72"/>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="68">
         <v>43972</v>
       </c>
@@ -4268,8 +4296,14 @@
         <v>119</v>
       </c>
       <c r="E65" s="72"/>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F65" t="s">
+        <v>148</v>
+      </c>
+      <c r="H65" s="70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="68">
         <v>43973</v>
       </c>
@@ -4277,8 +4311,17 @@
         <v>113</v>
       </c>
       <c r="E66" s="72"/>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F66" t="s">
+        <v>149</v>
+      </c>
+      <c r="G66">
+        <v>11000</v>
+      </c>
+      <c r="H66" s="70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="68">
         <v>43974</v>
       </c>
@@ -4286,8 +4329,14 @@
         <v>114</v>
       </c>
       <c r="E67" s="72"/>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F67" t="s">
+        <v>147</v>
+      </c>
+      <c r="H67" s="70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="68">
         <v>43975</v>
       </c>
@@ -4295,53 +4344,62 @@
         <v>115</v>
       </c>
       <c r="E68" s="72"/>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F68" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="68">
         <v>43976</v>
       </c>
       <c r="C69" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="D69" s="72" t="s">
-        <v>121</v>
+      <c r="D69" s="69" t="s">
+        <v>145</v>
       </c>
       <c r="E69" s="72"/>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="F69" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="68">
         <v>43977</v>
       </c>
       <c r="C70" s="67" t="s">
         <v>117</v>
       </c>
+      <c r="E70" s="72"/>
       <c r="F70" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="68">
         <v>43978</v>
       </c>
       <c r="C71" s="67" t="s">
         <v>118</v>
       </c>
+      <c r="E71" s="72"/>
       <c r="F71" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.35">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="68">
         <v>43979</v>
       </c>
       <c r="C72" s="67" t="s">
         <v>119</v>
       </c>
-      <c r="F72" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="D72" s="72" t="s">
+        <v>120</v>
+      </c>
+      <c r="E72" s="72"/>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="68">
         <v>43980</v>
       </c>
@@ -4349,42 +4407,42 @@
         <v>113</v>
       </c>
       <c r="F73" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="68"/>
       <c r="C74" s="67"/>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="68"/>
       <c r="C75" s="67"/>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="68"/>
       <c r="C76" s="67"/>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="68"/>
       <c r="C77" s="67"/>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="68"/>
       <c r="C78" s="67"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="68"/>
       <c r="C79" s="67"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="68"/>
       <c r="C80" s="67"/>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="68"/>
       <c r="C81" s="67"/>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="68"/>
       <c r="C82" s="67"/>
     </row>
@@ -4396,6 +4454,149 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30C54C2-F155-43D5-8CB0-E4CC882358D1}">
+  <dimension ref="B2:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R15" sqref="R15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" s="66" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="73">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C3" s="67">
+        <v>43959</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="73">
+        <v>0.5625</v>
+      </c>
+      <c r="C4" s="67">
+        <v>43959</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="73">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="C5" s="67">
+        <v>43959</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="73">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="C6" s="67">
+        <v>43959</v>
+      </c>
+      <c r="D6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="73">
+        <v>0.6875</v>
+      </c>
+      <c r="C7" s="67">
+        <v>43959</v>
+      </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="73">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C8" s="67">
+        <v>43960</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="73">
+        <v>0.5625</v>
+      </c>
+      <c r="C9" s="67">
+        <v>43960</v>
+      </c>
+      <c r="D9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="73">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="C10" s="67">
+        <v>43960</v>
+      </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="73">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="C11" s="67">
+        <v>43960</v>
+      </c>
+      <c r="D11">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="73">
+        <v>0.6875</v>
+      </c>
+      <c r="C12" s="67">
+        <v>43960</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A5C444-0508-4E0A-B501-37382ABBB1DA}">
   <dimension ref="A1:AI31"/>
   <sheetViews>
@@ -4403,15 +4604,15 @@
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.1796875" customWidth="1"/>
-    <col min="2" max="4" width="7.81640625" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" customWidth="1"/>
-    <col min="6" max="35" width="3.1796875" style="56" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="2" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="35" width="3.140625" style="56" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="str">
         <f>" Total hours: "&amp;(SUM(D3:D29) )</f>
         <v xml:space="preserve"> Total hours: 400</v>
@@ -4455,7 +4656,7 @@
       <c r="AH1" s="74"/>
       <c r="AI1" s="74"/>
     </row>
-    <row r="2" spans="1:35" ht="60" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:35" ht="60.75" x14ac:dyDescent="0.4">
       <c r="A2" s="23" t="s">
         <v>59</v>
       </c>
@@ -4559,7 +4760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>61</v>
       </c>
@@ -4598,7 +4799,7 @@
       <c r="AH3" s="40"/>
       <c r="AI3" s="41"/>
     </row>
-    <row r="4" spans="1:35" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>62</v>
       </c>
@@ -4649,7 +4850,7 @@
       <c r="AH4" s="31"/>
       <c r="AI4" s="43"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
         <v>29</v>
       </c>
@@ -4696,7 +4897,7 @@
       <c r="AH5" s="24"/>
       <c r="AI5" s="45"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="s">
         <v>23</v>
       </c>
@@ -4743,7 +4944,7 @@
       <c r="AH6" s="24"/>
       <c r="AI6" s="45"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
         <v>30</v>
       </c>
@@ -4790,7 +4991,7 @@
       <c r="AH7" s="24"/>
       <c r="AI7" s="45"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>28</v>
       </c>
@@ -4829,7 +5030,7 @@
       <c r="AH8" s="25"/>
       <c r="AI8" s="47"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
         <v>51</v>
       </c>
@@ -4876,7 +5077,7 @@
       <c r="AH9" s="24"/>
       <c r="AI9" s="45"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
         <v>52</v>
       </c>
@@ -4923,7 +5124,7 @@
       <c r="AH10" s="24"/>
       <c r="AI10" s="45"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>60</v>
       </c>
@@ -4970,7 +5171,7 @@
       <c r="AH11" s="24"/>
       <c r="AI11" s="45"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
         <v>56</v>
       </c>
@@ -5021,7 +5222,7 @@
       <c r="AH12" s="24"/>
       <c r="AI12" s="45"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>55</v>
       </c>
@@ -5076,7 +5277,7 @@
       <c r="AH13" s="24"/>
       <c r="AI13" s="45"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>58</v>
       </c>
@@ -5125,7 +5326,7 @@
       <c r="AH14" s="24"/>
       <c r="AI14" s="45"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>57</v>
       </c>
@@ -5174,7 +5375,7 @@
       <c r="AH15" s="24"/>
       <c r="AI15" s="45"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
         <v>54</v>
       </c>
@@ -5221,7 +5422,7 @@
       <c r="AH16" s="24"/>
       <c r="AI16" s="45"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
         <v>53</v>
       </c>
@@ -5270,7 +5471,7 @@
       <c r="AH17" s="24"/>
       <c r="AI17" s="45"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
         <v>64</v>
       </c>
@@ -5319,7 +5520,7 @@
       <c r="AH18" s="24"/>
       <c r="AI18" s="45"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
         <v>63</v>
       </c>
@@ -5368,7 +5569,7 @@
       <c r="AH19" s="24"/>
       <c r="AI19" s="45"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
         <v>13</v>
       </c>
@@ -5407,7 +5608,7 @@
       <c r="AH20" s="25"/>
       <c r="AI20" s="47"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
         <v>31</v>
       </c>
@@ -5492,7 +5693,7 @@
       <c r="AH21" s="24"/>
       <c r="AI21" s="45"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>37</v>
       </c>
@@ -5539,7 +5740,7 @@
       <c r="AH22" s="24"/>
       <c r="AI22" s="45"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>32</v>
       </c>
@@ -5586,7 +5787,7 @@
       <c r="AH23" s="24"/>
       <c r="AI23" s="45"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>33</v>
       </c>
@@ -5637,7 +5838,7 @@
       <c r="AH24" s="24"/>
       <c r="AI24" s="45"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>34</v>
       </c>
@@ -5690,7 +5891,7 @@
       <c r="AH25" s="24"/>
       <c r="AI25" s="45"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>35</v>
       </c>
@@ -5743,7 +5944,7 @@
       <c r="AH26" s="24"/>
       <c r="AI26" s="45"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
         <v>36</v>
       </c>
@@ -5792,7 +5993,7 @@
       <c r="AH27" s="24"/>
       <c r="AI27" s="45"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>38</v>
       </c>
@@ -5847,7 +6048,7 @@
       <c r="AH28" s="24"/>
       <c r="AI28" s="45"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
         <v>39</v>
       </c>
@@ -5896,11 +6097,11 @@
       <c r="AH29" s="51"/>
       <c r="AI29" s="54"/>
     </row>
-    <row r="30" spans="1:35" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="T30" s="24"/>
       <c r="U30" s="24"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>
@@ -6025,7 +6226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450C220C-F757-45A0-8919-C63FF95447E6}">
   <dimension ref="A1:AI31"/>
   <sheetViews>
@@ -6033,15 +6234,15 @@
       <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.1796875" customWidth="1"/>
-    <col min="2" max="4" width="7.81640625" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" customWidth="1"/>
-    <col min="6" max="35" width="3.1796875" style="21" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" customWidth="1"/>
+    <col min="2" max="4" width="7.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="35" width="3.140625" style="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="str">
         <f>" Total hours: "&amp;(SUM(D3:D29) )</f>
         <v xml:space="preserve"> Total hours: 400</v>
@@ -6085,7 +6286,7 @@
       <c r="AH1" s="74"/>
       <c r="AI1" s="74"/>
     </row>
-    <row r="2" spans="1:35" ht="60" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:35" ht="60.75" x14ac:dyDescent="0.4">
       <c r="A2" s="23" t="s">
         <v>59</v>
       </c>
@@ -6189,7 +6390,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>61</v>
       </c>
@@ -6228,7 +6429,7 @@
       <c r="AH3" s="40"/>
       <c r="AI3" s="41"/>
     </row>
-    <row r="4" spans="1:35" s="20" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>62</v>
       </c>
@@ -6279,7 +6480,7 @@
       <c r="AH4" s="31"/>
       <c r="AI4" s="43"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
         <v>29</v>
       </c>
@@ -6326,7 +6527,7 @@
       <c r="AH5" s="24"/>
       <c r="AI5" s="45"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="s">
         <v>23</v>
       </c>
@@ -6373,7 +6574,7 @@
       <c r="AH6" s="24"/>
       <c r="AI6" s="45"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
         <v>30</v>
       </c>
@@ -6421,7 +6622,7 @@
       <c r="AH7" s="24"/>
       <c r="AI7" s="45"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
         <v>28</v>
       </c>
@@ -6460,7 +6661,7 @@
       <c r="AH8" s="25"/>
       <c r="AI8" s="47"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
         <v>51</v>
       </c>
@@ -6507,7 +6708,7 @@
       <c r="AH9" s="24"/>
       <c r="AI9" s="45"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
         <v>52</v>
       </c>
@@ -6554,7 +6755,7 @@
       <c r="AH10" s="24"/>
       <c r="AI10" s="45"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>60</v>
       </c>
@@ -6603,7 +6804,7 @@
       <c r="AH11" s="24"/>
       <c r="AI11" s="45"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
         <v>56</v>
       </c>
@@ -6655,7 +6856,7 @@
       <c r="AH12" s="24"/>
       <c r="AI12" s="45"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" s="44" t="s">
         <v>55</v>
       </c>
@@ -6710,7 +6911,7 @@
       <c r="AH13" s="24"/>
       <c r="AI13" s="45"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>58</v>
       </c>
@@ -6759,7 +6960,7 @@
       <c r="AH14" s="24"/>
       <c r="AI14" s="45"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>57</v>
       </c>
@@ -6808,7 +7009,7 @@
       <c r="AH15" s="24"/>
       <c r="AI15" s="45"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" s="44" t="s">
         <v>54</v>
       </c>
@@ -6855,7 +7056,7 @@
       <c r="AH16" s="24"/>
       <c r="AI16" s="45"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" s="44" t="s">
         <v>53</v>
       </c>
@@ -6904,7 +7105,7 @@
       <c r="AH17" s="24"/>
       <c r="AI17" s="45"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
         <v>64</v>
       </c>
@@ -6954,7 +7155,7 @@
       <c r="AH18" s="24"/>
       <c r="AI18" s="45"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
         <v>63</v>
       </c>
@@ -7003,7 +7204,7 @@
       <c r="AH19" s="24"/>
       <c r="AI19" s="45"/>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" s="46" t="s">
         <v>13</v>
       </c>
@@ -7042,7 +7243,7 @@
       <c r="AH20" s="25"/>
       <c r="AI20" s="47"/>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
         <v>31</v>
       </c>
@@ -7127,7 +7328,7 @@
       <c r="AH21" s="24"/>
       <c r="AI21" s="45"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="48" t="s">
         <v>37</v>
       </c>
@@ -7174,7 +7375,7 @@
       <c r="AH22" s="24"/>
       <c r="AI22" s="45"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="48" t="s">
         <v>32</v>
       </c>
@@ -7221,7 +7422,7 @@
       <c r="AH23" s="24"/>
       <c r="AI23" s="45"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="48" t="s">
         <v>33</v>
       </c>
@@ -7269,7 +7470,7 @@
       <c r="AH24" s="24"/>
       <c r="AI24" s="45"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="48" t="s">
         <v>34</v>
       </c>
@@ -7322,7 +7523,7 @@
       <c r="AH25" s="24"/>
       <c r="AI25" s="45"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="48" t="s">
         <v>35</v>
       </c>
@@ -7375,7 +7576,7 @@
       <c r="AH26" s="24"/>
       <c r="AI26" s="45"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="48" t="s">
         <v>36</v>
       </c>
@@ -7424,7 +7625,7 @@
       <c r="AH27" s="24"/>
       <c r="AI27" s="45"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="48" t="s">
         <v>38</v>
       </c>
@@ -7479,7 +7680,7 @@
       <c r="AH28" s="24"/>
       <c r="AI28" s="45"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
         <v>39</v>
       </c>
@@ -7528,11 +7729,11 @@
       <c r="AH29" s="51"/>
       <c r="AI29" s="54"/>
     </row>
-    <row r="30" spans="1:35" ht="4.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="T30" s="24"/>
       <c r="U30" s="24"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>65</v>
       </c>

</xml_diff>